<commit_message>
- Change IO connector to 0.1 PTH right angled shrouded - Change USB connector - Change LEDs from 0603 to 0804 - Fix texts orientation
</commit_message>
<xml_diff>
--- a/hardware/v3.9/BusPirate-v3.9-SSOP.xlsx
+++ b/hardware/v3.9/BusPirate-v3.9-SSOP.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="BusPirate-v3.9-SSOP" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -34,9 +34,6 @@
     <t>Part no.</t>
   </si>
   <si>
-    <t>LED-0603</t>
-  </si>
-  <si>
     <t>LED</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>R5</t>
   </si>
   <si>
-    <t>RN1, RN2, RN3</t>
-  </si>
-  <si>
     <t>10K 4 Resistor array</t>
   </si>
   <si>
@@ -148,21 +142,9 @@
     <t>CON1</t>
   </si>
   <si>
-    <t>JST 1x10</t>
-  </si>
-  <si>
-    <t>2.0mm JST-PH series connector 10 pins</t>
-  </si>
-  <si>
     <t>CON2</t>
   </si>
   <si>
-    <t>JST 1x06</t>
-  </si>
-  <si>
-    <t>2.0mm JST-PH series connector 6 pins</t>
-  </si>
-  <si>
     <t>IC4</t>
   </si>
   <si>
@@ -194,6 +176,24 @@
   </si>
   <si>
     <t>PIC24FJ64GA002 16-bit General Purpose Flash Microcontroller</t>
+  </si>
+  <si>
+    <t>RN1, RN2, RN3, RN4</t>
+  </si>
+  <si>
+    <t>1x10</t>
+  </si>
+  <si>
+    <t>1x06</t>
+  </si>
+  <si>
+    <t>0.1" male header</t>
+  </si>
+  <si>
+    <t>0.1" shoruded right angled male header Molex 70553-0044</t>
+  </si>
+  <si>
+    <t>LED-0804</t>
   </si>
 </sst>
 </file>
@@ -1018,12 +1018,12 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" customWidth="1"/>
     <col min="7" max="7" width="114.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1053,19 +1053,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1073,19 +1073,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1093,19 +1093,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1113,19 +1113,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1133,19 +1133,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
       </c>
       <c r="E6">
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1153,19 +1153,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1173,19 +1173,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1193,19 +1193,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="E9">
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1213,19 +1213,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="E10">
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1233,19 +1233,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1253,19 +1253,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1273,19 +1273,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
         <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>34</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1293,19 +1293,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1313,19 +1313,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1333,19 +1333,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1353,19 +1353,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1373,19 +1373,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1393,19 +1393,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>